<commit_message>
update rd SDK library 1.0.448983
</commit_message>
<xml_diff>
--- a/android_studio/rdVEUISdk/rd_strings.xlsx
+++ b/android_studio/rdVEUISdk/rd_strings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547">
   <si>
     <t>name</t>
   </si>
@@ -4622,6 +4622,39 @@
   </si>
   <si>
     <t>Видео слишком короткое, не удалось захватить видео.</t>
+  </si>
+  <si>
+    <t>import_duration_limit</t>
+  </si>
+  <si>
+    <t>视频长度不能大于90秒</t>
+  </si>
+  <si>
+    <t>Can not export video with length more than 90s</t>
+  </si>
+  <si>
+    <t>导出视频长度不能大于90秒</t>
+  </si>
+  <si>
+    <t>影片時長超過 90 秒</t>
+  </si>
+  <si>
+    <t>La durée de la vidéo dépasse 90 secondes</t>
+  </si>
+  <si>
+    <t>Videolänge übersteigt 90 Sekunden</t>
+  </si>
+  <si>
+    <t>La lunghezza del video supera i 90 secondi</t>
+  </si>
+  <si>
+    <t>ビデオが90秒を超えています</t>
+  </si>
+  <si>
+    <t>동영상 길이가 90초를 초과합니다</t>
+  </si>
+  <si>
+    <t>Видео превышает 90 сек.</t>
   </si>
 </sst>
 </file>
@@ -4629,12 +4662,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4681,14 +4714,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4696,14 +4729,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4724,6 +4750,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -4731,9 +4780,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4749,38 +4837,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4788,44 +4852,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4846,19 +4872,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4870,7 +4938,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4888,13 +4986,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4906,127 +5046,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5055,54 +5081,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5114,6 +5092,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5144,6 +5131,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -5158,10 +5184,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5170,136 +5196,136 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5693,9 +5719,9 @@
   <dimension ref="A1:L773"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A551" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B453" sqref="B453"/>
+      <selection pane="bottomLeft" activeCell="B560" sqref="B560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.25"/>
@@ -12666,8 +12692,40 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="556" spans="2:2">
-      <c r="B556" s="8"/>
+    <row r="556" spans="1:11">
+      <c r="A556" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B556" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C556" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D556" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E556" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F556" t="s">
+        <v>1541</v>
+      </c>
+      <c r="G556" t="s">
+        <v>1542</v>
+      </c>
+      <c r="H556" t="s">
+        <v>1543</v>
+      </c>
+      <c r="I556" t="s">
+        <v>1544</v>
+      </c>
+      <c r="J556" t="s">
+        <v>1545</v>
+      </c>
+      <c r="K556" t="s">
+        <v>1546</v>
+      </c>
     </row>
     <row r="585" spans="2:2">
       <c r="B585" s="5"/>

</xml_diff>